<commit_message>
add alot of cart materials
</commit_message>
<xml_diff>
--- a/materials.xlsx
+++ b/materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="26140" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="16800" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Bridge M</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -138,6 +138,114 @@
   <si>
     <t>11.1V 500mah</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plane model Battery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.4 V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://c.b1yt.com/h.RzRBvE?cv=JcOMZDPYFw8&amp;sm=05822a</t>
+  </si>
+  <si>
+    <t>PCB Hole Board</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9 * 15 cm.    Gap 2.54mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://c.b1yt.com/h.RBB8vN?cv=YntWZDkLcZI&amp;sm=14debe</t>
+  </si>
+  <si>
+    <t>3M Thick Plastic tape</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://c.b1yt.com/h.RBBR5I?cv=peJzZDkoLYA&amp;sm=ad727b</t>
+  </si>
+  <si>
+    <t>http://c.b1yt.com/h.RBBLh7?cv=Cm61ZDko5ww&amp;sm=522d6b</t>
+  </si>
+  <si>
+    <t>Audi YoYo String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://c.b1yt.com/h.RBzd7v?cv=30hAZDkMt1P&amp;sm=cacddc </t>
+  </si>
+  <si>
+    <t>TowerPro 360Degree servo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 cm width</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://c.b1yt.com/h.RBBcoC?cv=jep3ZDkMRs9&amp;sm=61b866</t>
+  </si>
+  <si>
+    <t>2.7 * 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rubber Wheel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Diameter: 43 mm </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MG946R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://c.b1yt.com/h.RBy7i9?cv=tkwzZDkMXNM&amp;sm=52928b</t>
+  </si>
+  <si>
+    <t>12v 150rpm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N20 Moter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N20 stand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://c.b1yt.com/h.RBC0Mp?cv=ZeyhZDknEgF&amp;sm=1f14ff </t>
+  </si>
+  <si>
+    <t>http://c.b1yt.com/h.RBCLqG?cv=SR2TZDknZox&amp;sm=48cdf3</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">XTWduino nano V3.0 ATMEGA328P </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>改进开发板</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> arduino</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -184,10 +292,9 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b/>
-      <sz val="24"/>
-      <color rgb="FFFF4400"/>
-      <name val="Verdana"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="2">
@@ -212,11 +319,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -496,15 +602,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="52.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -559,10 +666,11 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>13.5</v>
+        <f>13.5*5</f>
+        <v>67.5</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
@@ -597,7 +705,7 @@
       <c r="E11">
         <v>10.6</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -614,48 +722,183 @@
       <c r="E12">
         <v>4</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>25</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0.99</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3">
-        <v>31</v>
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>38</v>
+      </c>
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="F23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>31</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>25</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
         <v>1.6</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F25" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>7.9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>3</v>
       </c>
     </row>
@@ -664,8 +907,17 @@
   <hyperlinks>
     <hyperlink ref="F11" r:id="rId1"/>
     <hyperlink ref="F12" r:id="rId2"/>
-    <hyperlink ref="F21" r:id="rId3"/>
-    <hyperlink ref="F20" r:id="rId4"/>
+    <hyperlink ref="F25" r:id="rId3"/>
+    <hyperlink ref="F24" r:id="rId4"/>
+    <hyperlink ref="F23" r:id="rId5"/>
+    <hyperlink ref="F26" r:id="rId6"/>
+    <hyperlink ref="F27" r:id="rId7"/>
+    <hyperlink ref="F28" r:id="rId8"/>
+    <hyperlink ref="F22" r:id="rId9"/>
+    <hyperlink ref="F21" r:id="rId10"/>
+    <hyperlink ref="F20" r:id="rId11"/>
+    <hyperlink ref="F19" r:id="rId12"/>
+    <hyperlink ref="F18" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update README and materials
</commit_message>
<xml_diff>
--- a/materials.xlsx
+++ b/materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="16800" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="16800" yWindow="440" windowWidth="16800" windowHeight="20480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -179,10 +179,6 @@
     <t>http://c.b1yt.com/h.RBzd7v?cv=30hAZDkMt1P&amp;sm=cacddc </t>
   </si>
   <si>
-    <t>TowerPro 360Degree servo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1 cm width</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -198,10 +194,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Diameter: 43 mm </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MG946R</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -214,10 +206,6 @@
   </si>
   <si>
     <t>N20 Moter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N20 stand</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -246,6 +234,18 @@
       </rPr>
       <t xml:space="preserve"> arduino</t>
     </r>
+  </si>
+  <si>
+    <t>N20 stand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Diameter: 43 mm </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TowerPro 360Degree servo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,7 +733,7 @@
     </row>
     <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -742,12 +742,12 @@
         <v>25</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -756,43 +756,43 @@
         <v>0.99</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -874,7 +874,7 @@
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27">
         <v>1</v>

</xml_diff>